<commit_message>
Fix error reading the excel file
</commit_message>
<xml_diff>
--- a/expt06.xlsx
+++ b/expt06.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Stockton university\Graduate assistantship\chemistry-experiments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A635FCA9-66C0-4134-B264-85034A4D0A54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C028A02-1780-41EA-A93C-DCA017A84D3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="500" activeTab="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="class data" sheetId="1" state="visible" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>Chemistry 2115:  General Chemistry Laboratory</t>
   </si>
@@ -424,219 +424,6 @@
   </si>
   <si>
     <t>D-6</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>0.105</t>
-  </si>
-  <si>
-    <t>26.718</t>
-  </si>
-  <si>
-    <t>26.807</t>
-  </si>
-  <si>
-    <t>0.0889999999999986</t>
-  </si>
-  <si>
-    <t>0.00056993974922651</t>
-  </si>
-  <si>
-    <t>0.000609130107453279</t>
-  </si>
-  <si>
-    <t>0.136</t>
-  </si>
-  <si>
-    <t>29.81</t>
-  </si>
-  <si>
-    <t>29.92</t>
-  </si>
-  <si>
-    <t>0.110000000000003</t>
-  </si>
-  <si>
-    <t>0.000738207675188623</t>
-  </si>
-  <si>
-    <t>0.000752857436178242</t>
-  </si>
-  <si>
-    <t>0.122</t>
-  </si>
-  <si>
-    <t>28.843</t>
-  </si>
-  <si>
-    <t>28.943</t>
-  </si>
-  <si>
-    <t>0.100000000000001</t>
-  </si>
-  <si>
-    <t>0.000662215708625088</t>
-  </si>
-  <si>
-    <t>0.00068441585107112</t>
-  </si>
-  <si>
-    <t>0.116</t>
-  </si>
-  <si>
-    <t>30.014</t>
-  </si>
-  <si>
-    <t>30.107</t>
-  </si>
-  <si>
-    <t>0.093</t>
-  </si>
-  <si>
-    <t>0.000629647722955002</t>
-  </si>
-  <si>
-    <t>0.000636506741496133</t>
-  </si>
-  <si>
-    <t>0.161</t>
-  </si>
-  <si>
-    <t>25.565</t>
-  </si>
-  <si>
-    <t>25.69</t>
-  </si>
-  <si>
-    <t>0.125</t>
-  </si>
-  <si>
-    <t>0.000873907615480649</t>
-  </si>
-  <si>
-    <t>0.000855519813838888</t>
-  </si>
-  <si>
-    <t>0.187</t>
-  </si>
-  <si>
-    <t>24.666</t>
-  </si>
-  <si>
-    <t>24.802</t>
-  </si>
-  <si>
-    <t>0.135999999999999</t>
-  </si>
-  <si>
-    <t>0.00101503555338436</t>
-  </si>
-  <si>
-    <t>0.000930805557456705</t>
-  </si>
-  <si>
-    <t>0.205</t>
-  </si>
-  <si>
-    <t>22.372</t>
-  </si>
-  <si>
-    <t>22.53</t>
-  </si>
-  <si>
-    <t>0.158000000000001</t>
-  </si>
-  <si>
-    <t>0.00111273951039462</t>
-  </si>
-  <si>
-    <t>0.00108137704469236</t>
-  </si>
-  <si>
-    <t>0.318</t>
-  </si>
-  <si>
-    <t>29.875</t>
-  </si>
-  <si>
-    <t>30.047</t>
-  </si>
-  <si>
-    <t>0.172000000000001</t>
-  </si>
-  <si>
-    <t>0.00172610324051457</t>
-  </si>
-  <si>
-    <t>0.00117719526384231</t>
-  </si>
-  <si>
-    <t>0.257</t>
-  </si>
-  <si>
-    <t>30.273</t>
-  </si>
-  <si>
-    <t>30.446</t>
-  </si>
-  <si>
-    <t>0.173000000000002</t>
-  </si>
-  <si>
-    <t>0.00139499538620203</t>
-  </si>
-  <si>
-    <t>0.00118403942235303</t>
-  </si>
-  <si>
-    <t>0.25</t>
-  </si>
-  <si>
-    <t>20.785</t>
-  </si>
-  <si>
-    <t>20.962</t>
-  </si>
-  <si>
-    <t>0.177</t>
-  </si>
-  <si>
-    <t>0.00135699940292026</t>
-  </si>
-  <si>
-    <t>0.00121141605639586</t>
-  </si>
-  <si>
-    <t>0.213</t>
-  </si>
-  <si>
-    <t>22.316</t>
-  </si>
-  <si>
-    <t>22.486</t>
-  </si>
-  <si>
-    <t>0.170000000000002</t>
-  </si>
-  <si>
-    <t>0.00115616349128806</t>
-  </si>
-  <si>
-    <t>0.0011635069468209</t>
-  </si>
-  <si>
-    <t>0.219</t>
-  </si>
-  <si>
-    <t>29.898</t>
-  </si>
-  <si>
-    <t>30.07</t>
-  </si>
-  <si>
-    <t>0.00118873147695815</t>
   </si>
 </sst>
 </file>
@@ -1138,8 +925,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1609,8 +1396,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Add remove empty lines
</commit_message>
<xml_diff>
--- a/expt06.xlsx
+++ b/expt06.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Stockton university\Graduate assistantship\chemistry-experiments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{333D2B85-ED14-489D-AD92-FD23D0677F8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1723829-E454-48E7-9BD7-0CAE2F3B8BC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>Chemistry 2115:  General Chemistry Laboratory</t>
   </si>
@@ -424,33 +424,6 @@
   </si>
   <si>
     <t>D-6</t>
-  </si>
-  <si>
-    <t>26.718</t>
-  </si>
-  <si>
-    <t>0.08</t>
-  </si>
-  <si>
-    <t>0.079</t>
-  </si>
-  <si>
-    <t>25.005</t>
-  </si>
-  <si>
-    <t>-25.005</t>
-  </si>
-  <si>
-    <t>25.001</t>
-  </si>
-  <si>
-    <t>-25.001</t>
-  </si>
-  <si>
-    <t>26</t>
-  </si>
-  <si>
-    <t>27</t>
   </si>
 </sst>
 </file>
@@ -955,8 +928,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1085,9 +1058,7 @@
       <c r="A10" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="33" t="s">
-        <v>37</v>
-      </c>
+      <c r="B10" s="33"/>
       <c r="C10" s="33"/>
       <c r="D10" s="33"/>
       <c r="E10" s="29"/>
@@ -1099,10 +1070,14 @@
         <v>14</v>
       </c>
       <c r="B11" s="34">
-        <v>-0.05</v>
-      </c>
-      <c r="C11" s="34"/>
-      <c r="D11" s="34"/>
+        <v>0.105</v>
+      </c>
+      <c r="C11" s="34">
+        <v>26.718</v>
+      </c>
+      <c r="D11" s="34">
+        <v>26.806999999999999</v>
+      </c>
       <c r="E11" s="26"/>
       <c r="F11" s="26"/>
       <c r="G11" s="26"/>
@@ -1111,11 +1086,15 @@
       <c r="A12" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="C12" s="33"/>
-      <c r="D12" s="33"/>
+      <c r="B12" s="33">
+        <v>0.13600000000000001</v>
+      </c>
+      <c r="C12" s="33">
+        <v>29.81</v>
+      </c>
+      <c r="D12" s="33">
+        <v>29.92</v>
+      </c>
       <c r="E12" s="29"/>
       <c r="F12" s="29"/>
       <c r="G12" s="30"/>
@@ -1124,11 +1103,15 @@
       <c r="A13" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="32"/>
-      <c r="C13" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="D13" s="32"/>
+      <c r="B13" s="32">
+        <v>0.122</v>
+      </c>
+      <c r="C13" s="32">
+        <v>28.843</v>
+      </c>
+      <c r="D13" s="32">
+        <v>28.943000000000001</v>
+      </c>
       <c r="E13" s="27"/>
       <c r="F13" s="31"/>
       <c r="G13" s="31"/>
@@ -1137,11 +1120,15 @@
       <c r="A14" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="33"/>
-      <c r="C14" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="D14" s="33"/>
+      <c r="B14" s="33">
+        <v>0.11600000000000001</v>
+      </c>
+      <c r="C14" s="33">
+        <v>30.013999999999999</v>
+      </c>
+      <c r="D14" s="33">
+        <v>30.106999999999999</v>
+      </c>
       <c r="E14" s="29"/>
       <c r="F14" s="29"/>
       <c r="G14" s="30"/>
@@ -1152,9 +1139,7 @@
       </c>
       <c r="B15" s="34"/>
       <c r="C15" s="34"/>
-      <c r="D15" s="34" t="s">
-        <v>41</v>
-      </c>
+      <c r="D15" s="34"/>
       <c r="E15" s="27"/>
       <c r="F15" s="31"/>
       <c r="G15" s="31"/>
@@ -1163,12 +1148,14 @@
       <c r="A16" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="33"/>
-      <c r="C16" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="D16" s="33" t="s">
-        <v>41</v>
+      <c r="B16" s="33">
+        <v>0.161</v>
+      </c>
+      <c r="C16" s="33">
+        <v>25.565000000000001</v>
+      </c>
+      <c r="D16" s="33">
+        <v>25.69</v>
       </c>
       <c r="E16" s="29"/>
       <c r="F16" s="29"/>
@@ -1179,12 +1166,8 @@
         <v>20</v>
       </c>
       <c r="B17" s="32"/>
-      <c r="C17" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="D17" s="32" t="s">
-        <v>42</v>
-      </c>
+      <c r="C17" s="32"/>
+      <c r="D17" s="32"/>
       <c r="E17" s="27"/>
       <c r="F17" s="31"/>
       <c r="G17" s="31"/>
@@ -1194,12 +1177,8 @@
         <v>21</v>
       </c>
       <c r="B18" s="33"/>
-      <c r="C18" s="33" t="s">
-        <v>43</v>
-      </c>
-      <c r="D18" s="33" t="s">
-        <v>41</v>
-      </c>
+      <c r="C18" s="33"/>
+      <c r="D18" s="33"/>
       <c r="E18" s="29"/>
       <c r="F18" s="29"/>
       <c r="G18" s="30"/>
@@ -1208,12 +1187,14 @@
       <c r="A19" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="B19" s="32"/>
-      <c r="C19" s="32" t="s">
-        <v>43</v>
-      </c>
-      <c r="D19" s="32" t="s">
-        <v>42</v>
+      <c r="B19" s="32">
+        <v>0.187</v>
+      </c>
+      <c r="C19" s="32">
+        <v>24.666</v>
+      </c>
+      <c r="D19" s="32">
+        <v>24.802</v>
       </c>
       <c r="E19" s="27"/>
       <c r="F19" s="31"/>
@@ -1223,12 +1204,14 @@
       <c r="A20" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="B20" s="33"/>
-      <c r="C20" s="33" t="s">
-        <v>43</v>
-      </c>
-      <c r="D20" s="33" t="s">
-        <v>44</v>
+      <c r="B20" s="33">
+        <v>0.20499999999999999</v>
+      </c>
+      <c r="C20" s="33">
+        <v>22.372</v>
+      </c>
+      <c r="D20" s="33">
+        <v>22.53</v>
       </c>
       <c r="E20" s="29"/>
       <c r="F20" s="29"/>
@@ -1260,6 +1243,15 @@
       <c r="A23" s="26" t="s">
         <v>26</v>
       </c>
+      <c r="B23" s="26">
+        <v>0.318</v>
+      </c>
+      <c r="C23" s="26">
+        <v>29.875</v>
+      </c>
+      <c r="D23" s="26">
+        <v>30.047000000000001</v>
+      </c>
       <c r="E23" s="27"/>
       <c r="F23" s="31"/>
       <c r="G23" s="31"/>
@@ -1268,9 +1260,15 @@
       <c r="A24" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="B24" s="33"/>
-      <c r="C24" s="33"/>
-      <c r="D24" s="33"/>
+      <c r="B24" s="33">
+        <v>0.25700000000000001</v>
+      </c>
+      <c r="C24" s="33">
+        <v>30.273</v>
+      </c>
+      <c r="D24" s="33">
+        <v>30.446000000000002</v>
+      </c>
       <c r="E24" s="29"/>
       <c r="F24" s="29"/>
       <c r="G24" s="30"/>
@@ -1323,9 +1321,15 @@
       <c r="A29" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="B29" s="32"/>
-      <c r="C29" s="32"/>
-      <c r="D29" s="32"/>
+      <c r="B29" s="32">
+        <v>0.25</v>
+      </c>
+      <c r="C29" s="32">
+        <v>20.785</v>
+      </c>
+      <c r="D29" s="32">
+        <v>20.962</v>
+      </c>
       <c r="E29" s="27"/>
       <c r="F29" s="31"/>
       <c r="G29" s="31"/>
@@ -1334,9 +1338,15 @@
       <c r="A30" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="B30" s="33"/>
-      <c r="C30" s="33"/>
-      <c r="D30" s="33"/>
+      <c r="B30" s="33">
+        <v>0.21299999999999999</v>
+      </c>
+      <c r="C30" s="33">
+        <v>22.315999999999999</v>
+      </c>
+      <c r="D30" s="33">
+        <v>22.486000000000001</v>
+      </c>
       <c r="E30" s="29"/>
       <c r="F30" s="29"/>
       <c r="G30" s="30"/>
@@ -1357,13 +1367,13 @@
         <v>35</v>
       </c>
       <c r="B32" s="33">
-        <v>8.1000000000000003E-2</v>
-      </c>
-      <c r="C32" s="33" t="s">
-        <v>36</v>
+        <v>0.219</v>
+      </c>
+      <c r="C32" s="33">
+        <v>29.898</v>
       </c>
       <c r="D32" s="33">
-        <v>26.801511822178799</v>
+        <v>30.07</v>
       </c>
       <c r="E32" s="29"/>
       <c r="F32" s="29"/>
@@ -1389,8 +1399,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1549,7 +1559,7 @@
       </c>
       <c r="B10" s="33" t="inlineStr">
         <is>
-          <t>0.08</t>
+          <t/>
         </is>
       </c>
       <c r="C10" s="33" t="inlineStr">
@@ -1569,7 +1579,7 @@
       </c>
       <c r="F10" s="29" t="inlineStr">
         <is>
-          <t>0.00043424</t>
+          <t/>
         </is>
       </c>
       <c r="G10" s="30" t="inlineStr">
@@ -1586,32 +1596,32 @@
       </c>
       <c r="B11" s="34" t="inlineStr">
         <is>
-          <t>-0.05</t>
+          <t>0.105</t>
         </is>
       </c>
       <c r="C11" s="34" t="inlineStr">
         <is>
-          <t/>
+          <t>26.718</t>
         </is>
       </c>
       <c r="D11" s="34" t="inlineStr">
         <is>
-          <t/>
+          <t>26.807</t>
         </is>
       </c>
       <c r="E11" s="26" t="inlineStr">
         <is>
-          <t/>
+          <t>0.089</t>
         </is>
       </c>
       <c r="F11" s="26" t="inlineStr">
         <is>
-          <t/>
+          <t>0.00056994</t>
         </is>
       </c>
       <c r="G11" s="26" t="inlineStr">
         <is>
-          <t/>
+          <t>0.00060913</t>
         </is>
       </c>
     </row>
@@ -1623,32 +1633,32 @@
       </c>
       <c r="B12" s="33" t="inlineStr">
         <is>
-          <t>0.079</t>
+          <t>0.136</t>
         </is>
       </c>
       <c r="C12" s="33" t="inlineStr">
         <is>
-          <t/>
+          <t>29.81</t>
         </is>
       </c>
       <c r="D12" s="33" t="inlineStr">
         <is>
-          <t/>
+          <t>29.92</t>
         </is>
       </c>
       <c r="E12" s="29" t="inlineStr">
         <is>
-          <t/>
+          <t>0.11</t>
         </is>
       </c>
       <c r="F12" s="29" t="inlineStr">
         <is>
-          <t/>
+          <t>0.000738208</t>
         </is>
       </c>
       <c r="G12" s="30" t="inlineStr">
         <is>
-          <t/>
+          <t>0.000752857</t>
         </is>
       </c>
     </row>
@@ -1660,32 +1670,32 @@
       </c>
       <c r="B13" s="32" t="inlineStr">
         <is>
-          <t/>
+          <t>0.122</t>
         </is>
       </c>
       <c r="C13" s="32" t="inlineStr">
         <is>
-          <t>25.005</t>
+          <t>28.843</t>
         </is>
       </c>
       <c r="D13" s="32" t="inlineStr">
         <is>
-          <t/>
+          <t>28.943</t>
         </is>
       </c>
       <c r="E13" s="27" t="inlineStr">
         <is>
-          <t/>
+          <t>0.1</t>
         </is>
       </c>
       <c r="F13" s="31" t="inlineStr">
         <is>
-          <t/>
+          <t>0.000662216</t>
         </is>
       </c>
       <c r="G13" s="31" t="inlineStr">
         <is>
-          <t/>
+          <t>0.000684416</t>
         </is>
       </c>
     </row>
@@ -1697,32 +1707,32 @@
       </c>
       <c r="B14" s="33" t="inlineStr">
         <is>
-          <t/>
+          <t>0.116</t>
         </is>
       </c>
       <c r="C14" s="33" t="inlineStr">
         <is>
-          <t>-25.005</t>
+          <t>30.014</t>
         </is>
       </c>
       <c r="D14" s="33" t="inlineStr">
         <is>
-          <t/>
+          <t>30.107</t>
         </is>
       </c>
       <c r="E14" s="29" t="inlineStr">
         <is>
-          <t/>
+          <t>0.093</t>
         </is>
       </c>
       <c r="F14" s="29" t="inlineStr">
         <is>
-          <t/>
+          <t>0.000629648</t>
         </is>
       </c>
       <c r="G14" s="30" t="inlineStr">
         <is>
-          <t/>
+          <t>0.000636507</t>
         </is>
       </c>
     </row>
@@ -1744,7 +1754,7 @@
       </c>
       <c r="D15" s="34" t="inlineStr">
         <is>
-          <t>25.001</t>
+          <t/>
         </is>
       </c>
       <c r="E15" s="27" t="inlineStr">
@@ -1771,32 +1781,32 @@
       </c>
       <c r="B16" s="33" t="inlineStr">
         <is>
-          <t/>
+          <t>0.161</t>
         </is>
       </c>
       <c r="C16" s="33" t="inlineStr">
         <is>
-          <t>-25.005</t>
+          <t>25.565</t>
         </is>
       </c>
       <c r="D16" s="33" t="inlineStr">
         <is>
-          <t>25.001</t>
+          <t>25.69</t>
         </is>
       </c>
       <c r="E16" s="29" t="inlineStr">
         <is>
-          <t/>
+          <t>0.125</t>
         </is>
       </c>
       <c r="F16" s="29" t="inlineStr">
         <is>
-          <t/>
+          <t>0.000873908</t>
         </is>
       </c>
       <c r="G16" s="30" t="inlineStr">
         <is>
-          <t/>
+          <t>0.00085552</t>
         </is>
       </c>
     </row>
@@ -1813,12 +1823,12 @@
       </c>
       <c r="C17" s="32" t="inlineStr">
         <is>
-          <t>-25.005</t>
+          <t/>
         </is>
       </c>
       <c r="D17" s="32" t="inlineStr">
         <is>
-          <t>-25.001</t>
+          <t/>
         </is>
       </c>
       <c r="E17" s="27" t="inlineStr">
@@ -1850,12 +1860,12 @@
       </c>
       <c r="C18" s="33" t="inlineStr">
         <is>
-          <t>26</t>
+          <t/>
         </is>
       </c>
       <c r="D18" s="33" t="inlineStr">
         <is>
-          <t>25.001</t>
+          <t/>
         </is>
       </c>
       <c r="E18" s="29" t="inlineStr">
@@ -1882,32 +1892,32 @@
       </c>
       <c r="B19" s="32" t="inlineStr">
         <is>
-          <t/>
+          <t>0.187</t>
         </is>
       </c>
       <c r="C19" s="32" t="inlineStr">
         <is>
-          <t>26</t>
+          <t>24.666</t>
         </is>
       </c>
       <c r="D19" s="32" t="inlineStr">
         <is>
-          <t>-25.001</t>
+          <t>24.802</t>
         </is>
       </c>
       <c r="E19" s="27" t="inlineStr">
         <is>
-          <t/>
+          <t>0.136</t>
         </is>
       </c>
       <c r="F19" s="31" t="inlineStr">
         <is>
-          <t/>
+          <t>0.001015036</t>
         </is>
       </c>
       <c r="G19" s="31" t="inlineStr">
         <is>
-          <t/>
+          <t>0.000930806</t>
         </is>
       </c>
     </row>
@@ -1919,32 +1929,32 @@
       </c>
       <c r="B20" s="33" t="inlineStr">
         <is>
-          <t/>
+          <t>0.205</t>
         </is>
       </c>
       <c r="C20" s="33" t="inlineStr">
         <is>
-          <t>26</t>
+          <t>22.372</t>
         </is>
       </c>
       <c r="D20" s="33" t="inlineStr">
         <is>
-          <t>27</t>
+          <t>22.53</t>
         </is>
       </c>
       <c r="E20" s="29" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0.158</t>
         </is>
       </c>
       <c r="F20" s="29" t="inlineStr">
         <is>
-          <t/>
+          <t>0.00111274</t>
         </is>
       </c>
       <c r="G20" s="30" t="inlineStr">
         <is>
-          <t>0.006844159</t>
+          <t>0.001081377</t>
         </is>
       </c>
     </row>
@@ -2028,34 +2038,34 @@
           <t>C-3</t>
         </is>
       </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t/>
+      <c r="B23" s="26" t="inlineStr">
+        <is>
+          <t>0.318</t>
+        </is>
+      </c>
+      <c r="C23" s="26" t="inlineStr">
+        <is>
+          <t>29.875</t>
+        </is>
+      </c>
+      <c r="D23" s="26" t="inlineStr">
+        <is>
+          <t>30.047</t>
         </is>
       </c>
       <c r="E23" s="27" t="inlineStr">
         <is>
-          <t/>
+          <t>0.172</t>
         </is>
       </c>
       <c r="F23" s="31" t="inlineStr">
         <is>
-          <t/>
+          <t>0.001726103</t>
         </is>
       </c>
       <c r="G23" s="31" t="inlineStr">
         <is>
-          <t/>
+          <t>0.001177195</t>
         </is>
       </c>
     </row>
@@ -2067,32 +2077,32 @@
       </c>
       <c r="B24" s="33" t="inlineStr">
         <is>
-          <t/>
+          <t>0.257</t>
         </is>
       </c>
       <c r="C24" s="33" t="inlineStr">
         <is>
-          <t/>
+          <t>30.273</t>
         </is>
       </c>
       <c r="D24" s="33" t="inlineStr">
         <is>
-          <t/>
+          <t>30.446</t>
         </is>
       </c>
       <c r="E24" s="29" t="inlineStr">
         <is>
-          <t/>
+          <t>0.173</t>
         </is>
       </c>
       <c r="F24" s="29" t="inlineStr">
         <is>
-          <t/>
+          <t>0.001394995</t>
         </is>
       </c>
       <c r="G24" s="30" t="inlineStr">
         <is>
-          <t/>
+          <t>0.001184039</t>
         </is>
       </c>
     </row>
@@ -2252,32 +2262,32 @@
       </c>
       <c r="B29" s="32" t="inlineStr">
         <is>
-          <t/>
+          <t>0.25</t>
         </is>
       </c>
       <c r="C29" s="32" t="inlineStr">
         <is>
-          <t/>
+          <t>20.785</t>
         </is>
       </c>
       <c r="D29" s="32" t="inlineStr">
         <is>
-          <t/>
+          <t>20.962</t>
         </is>
       </c>
       <c r="E29" s="27" t="inlineStr">
         <is>
-          <t/>
+          <t>0.177</t>
         </is>
       </c>
       <c r="F29" s="31" t="inlineStr">
         <is>
-          <t/>
+          <t>0.001356999</t>
         </is>
       </c>
       <c r="G29" s="31" t="inlineStr">
         <is>
-          <t/>
+          <t>0.001211416</t>
         </is>
       </c>
     </row>
@@ -2289,32 +2299,32 @@
       </c>
       <c r="B30" s="33" t="inlineStr">
         <is>
-          <t/>
+          <t>0.213</t>
         </is>
       </c>
       <c r="C30" s="33" t="inlineStr">
         <is>
-          <t/>
+          <t>22.316</t>
         </is>
       </c>
       <c r="D30" s="33" t="inlineStr">
         <is>
-          <t/>
+          <t>22.486</t>
         </is>
       </c>
       <c r="E30" s="29" t="inlineStr">
         <is>
-          <t/>
+          <t>0.17</t>
         </is>
       </c>
       <c r="F30" s="29" t="inlineStr">
         <is>
-          <t/>
+          <t>0.001156163</t>
         </is>
       </c>
       <c r="G30" s="30" t="inlineStr">
         <is>
-          <t/>
+          <t>0.001163507</t>
         </is>
       </c>
     </row>
@@ -2363,32 +2373,32 @@
       </c>
       <c r="B32" s="33" t="inlineStr">
         <is>
-          <t>0.081</t>
+          <t>0.219</t>
         </is>
       </c>
       <c r="C32" s="33" t="inlineStr">
         <is>
-          <t>26.718</t>
+          <t>29.898</t>
         </is>
       </c>
       <c r="D32" s="33" t="inlineStr">
         <is>
-          <t>26.8015118221788</t>
+          <t>30.07</t>
         </is>
       </c>
       <c r="E32" s="29" t="inlineStr">
         <is>
-          <t>0.083511822</t>
+          <t>0.172</t>
         </is>
       </c>
       <c r="F32" s="29" t="inlineStr">
         <is>
-          <t>0.000439668</t>
+          <t>0.001188731</t>
         </is>
       </c>
       <c r="G32" s="30" t="inlineStr">
         <is>
-          <t>0.000571568</t>
+          <t>0.001177195</t>
         </is>
       </c>
     </row>

</xml_diff>